<commit_message>
pt3ex2 work in progress
</commit_message>
<xml_diff>
--- a/part3/exercise2/solutions/Esperimento content-to-form.xlsx
+++ b/part3/exercise2/solutions/Esperimento content-to-form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzotabasso/Desktop/University/TLN/Progetto/19-20/tln-1920/part3/exercise2/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzotabasso/Desktop/University/TLN/Progetto/19-20/tln-1920/part3/exercise2/solutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE24F7B-CA3D-8E45-B7B8-4E8A86149348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBF78B5-7ED7-254C-BE9C-66EE02642AEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18700" yWindow="-5140" windowWidth="18700" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -30054,13 +30054,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F751F1A-C83D-9142-8866-7E8B2171D954}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>

</xml_diff>